<commit_message>
Tweak to pivot experiment.
</commit_message>
<xml_diff>
--- a/methane.xlsx
+++ b/methane.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rolyp/Repo/explorable-viz/fluid-example-ipcc-ar6-01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA9B75C-51F7-544A-8E66-0ACC2C8DCAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4440C23-C380-144D-86E4-BFD5D22A144A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
   <si>
     <t>year</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>Grand Total</t>
-  </si>
-  <si>
-    <t>Count of  type</t>
   </si>
   <si>
     <t>Sum of  emissions</t>
@@ -555,13 +552,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -774,7 +775,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable6" cacheId="22" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:C6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <location ref="A3:B31" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
       <items count="3">
@@ -783,7 +784,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField dataField="1" showAll="0">
+    <pivotField axis="axisRow" showAll="0">
       <items count="11">
         <item x="0"/>
         <item x="1"/>
@@ -800,34 +801,101 @@
     </pivotField>
     <pivotField dataField="1" showAll="0"/>
   </pivotFields>
-  <rowFields count="1">
+  <rowFields count="2">
+    <field x="1"/>
     <field x="0"/>
   </rowFields>
-  <rowItems count="3">
+  <rowItems count="28">
     <i>
       <x/>
     </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
     <i>
       <x v="1"/>
     </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
   </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
+  <colItems count="1">
+    <i/>
   </colItems>
-  <dataFields count="2">
+  <dataFields count="1">
     <dataField name="Sum of  emissions" fld="2" baseField="0" baseItem="0"/>
-    <dataField name="Count of  type" fld="1" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -1381,7 +1449,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:C6"/>
+  <dimension ref="A3:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -1389,7 +1457,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
@@ -1401,48 +1469,236 @@
     <col min="10" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>4.2393926799999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
         <v>2070</v>
       </c>
-      <c r="B4">
-        <v>255.90313097000001</v>
-      </c>
-      <c r="C4">
+      <c r="B5" s="4">
+        <v>2.0805021099999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>2080</v>
+      </c>
+      <c r="B6" s="4">
+        <v>2.1588905700000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4">
+        <v>220.00880386</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>2070</v>
+      </c>
+      <c r="B8" s="4">
+        <v>109.93855666</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>2080</v>
+      </c>
+      <c r="B9" s="4">
+        <v>110.0702472</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="4">
+        <v>245.14098553000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>2070</v>
+      </c>
+      <c r="B11" s="4">
+        <v>125.14149136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>2080</v>
+      </c>
+      <c r="B12" s="4">
+        <v>119.99949417000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.91136978999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>2070</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0.45346383000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
+        <v>2080</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.45790596</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="4">
+        <v>6.8987241499999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>2070</v>
+      </c>
+      <c r="B17" s="4">
+        <v>3.5271644100000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>2080</v>
+      </c>
+      <c r="B18" s="4">
+        <v>3.3715597399999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="4">
+        <v>0.19988065999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>2070</v>
+      </c>
+      <c r="B20" s="4">
+        <v>0.10005683</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <v>2080</v>
+      </c>
+      <c r="B21" s="4">
+        <v>9.9823830000000002E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="B22" s="4">
+        <v>0.33393673000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="5">
+        <v>2070</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0.21893571000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
         <v>2080</v>
       </c>
-      <c r="B5">
-        <v>249.84379932000002</v>
-      </c>
-      <c r="C5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="B24" s="4">
+        <v>0.11500102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="4">
+        <v>0.13648504</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="5">
+        <v>2070</v>
+      </c>
+      <c r="B26" s="4">
+        <v>6.8173040000000004E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="5">
+        <v>2080</v>
+      </c>
+      <c r="B27" s="4">
+        <v>6.8311999999999998E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="4">
+        <v>27.87735185</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="5">
+        <v>2070</v>
+      </c>
+      <c r="B29" s="4">
+        <v>14.374787019999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
+        <v>2080</v>
+      </c>
+      <c r="B30" s="4">
+        <v>13.502564830000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B6">
+      <c r="B31" s="4">
         <v>505.74693028999997</v>
-      </c>
-      <c r="C6">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>